<commit_message>
Fix Plat Total Defects
</commit_message>
<xml_diff>
--- a/BasePlatform/Haizir Analysis/BackUp/LastMonth/ServicesDefects_Post_v8.1v8.2v8.3_Release2021_2022.xlsx
+++ b/BasePlatform/Haizir Analysis/BackUp/LastMonth/ServicesDefects_Post_v8.1v8.2v8.3_Release2021_2022.xlsx
@@ -25,15 +25,15 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
-    <pivotCache cacheId="1" r:id="rId8"/>
-    <pivotCache cacheId="2" r:id="rId9"/>
+    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="3" r:id="rId8"/>
+    <pivotCache cacheId="4" r:id="rId9"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6452" uniqueCount="1901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6563" uniqueCount="1930">
   <si>
     <t>Issue Type</t>
   </si>
@@ -5913,6 +5913,93 @@
   </si>
   <si>
     <t>Follow_Up</t>
+  </si>
+  <si>
+    <t>PLAT-24288</t>
+  </si>
+  <si>
+    <t>BOTW NGDE- Issue with Customer Entity profiles- Bulk profiling throws error</t>
+  </si>
+  <si>
+    <t>Possible project config issues</t>
+  </si>
+  <si>
+    <t>PLAT-24289</t>
+  </si>
+  <si>
+    <t>JBoss MDB Listener Handling</t>
+  </si>
+  <si>
+    <t>Require project-leve fix or future enhancement</t>
+  </si>
+  <si>
+    <t>PLAT-24291</t>
+  </si>
+  <si>
+    <t>CLONE - [SWIFT MX] Error - Non Alerted : DATA_SOURCE_SWIFT_MX_NO_HIT</t>
+  </si>
+  <si>
+    <t>PLAT-24292</t>
+  </si>
+  <si>
+    <t>No Hit SWIFT MT message with 32A tag is not stored when amount value with decimal</t>
+  </si>
+  <si>
+    <t>PLAT-24293</t>
+  </si>
+  <si>
+    <t>Although data label can be used in detection logic it's throwing an error while processing</t>
+  </si>
+  <si>
+    <t>Require enhancement</t>
+  </si>
+  <si>
+    <t>PLAT-24298</t>
+  </si>
+  <si>
+    <t>[FTB-412] - Active sessions screen not displaying correctly</t>
+  </si>
+  <si>
+    <t>User logging issue</t>
+  </si>
+  <si>
+    <t>PLAT-24301</t>
+  </si>
+  <si>
+    <t>Detections not generated when one of DATECOMPARE function parameters is null</t>
+  </si>
+  <si>
+    <t>Test gap in AML Detection</t>
+  </si>
+  <si>
+    <t>PLAT-24302</t>
+  </si>
+  <si>
+    <t>[ZKB] Total value profile not calculated properly when no past profiles created</t>
+  </si>
+  <si>
+    <t>PLAT-24303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMT messages not screened completely by OOTB SWIFT MX parser in NR V8 </t>
+  </si>
+  <si>
+    <t>SWIFTMX originally did not cover CAMT message. However, the new change has been backported to 8.4 version</t>
+  </si>
+  <si>
+    <t>PLAT-24305</t>
+  </si>
+  <si>
+    <t>Complete Message is not displayed for TransferWise Batch alert that using XML Transformer</t>
+  </si>
+  <si>
+    <t>PLAT-24306</t>
+  </si>
+  <si>
+    <t>[OCBC-280] AMLKYC: NetReveal Full vs Delta Screening Finished but Status not updated in Database</t>
+  </si>
+  <si>
+    <t>Intermittent issue and possible test gap</t>
   </si>
 </sst>
 </file>
@@ -23243,7 +23330,789 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5" rowHeaderCaption="Analysis Category">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10" rowHeaderCaption="Analysis Category">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="16">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="368">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="103"/>
+        <item x="104"/>
+        <item x="105"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="109"/>
+        <item x="110"/>
+        <item x="111"/>
+        <item x="112"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="120"/>
+        <item x="121"/>
+        <item x="122"/>
+        <item x="123"/>
+        <item x="124"/>
+        <item x="125"/>
+        <item x="126"/>
+        <item x="127"/>
+        <item x="128"/>
+        <item x="129"/>
+        <item x="130"/>
+        <item x="131"/>
+        <item x="132"/>
+        <item x="133"/>
+        <item x="134"/>
+        <item x="135"/>
+        <item x="136"/>
+        <item x="137"/>
+        <item x="138"/>
+        <item x="139"/>
+        <item x="140"/>
+        <item x="141"/>
+        <item x="142"/>
+        <item x="143"/>
+        <item x="144"/>
+        <item x="145"/>
+        <item x="146"/>
+        <item x="147"/>
+        <item x="148"/>
+        <item x="149"/>
+        <item x="150"/>
+        <item x="151"/>
+        <item x="152"/>
+        <item x="153"/>
+        <item x="154"/>
+        <item x="155"/>
+        <item x="156"/>
+        <item x="157"/>
+        <item x="158"/>
+        <item x="159"/>
+        <item x="160"/>
+        <item x="161"/>
+        <item x="162"/>
+        <item x="163"/>
+        <item x="164"/>
+        <item x="165"/>
+        <item x="166"/>
+        <item x="167"/>
+        <item x="168"/>
+        <item x="169"/>
+        <item x="170"/>
+        <item x="171"/>
+        <item x="172"/>
+        <item x="173"/>
+        <item x="174"/>
+        <item x="175"/>
+        <item x="176"/>
+        <item x="177"/>
+        <item x="178"/>
+        <item x="179"/>
+        <item x="180"/>
+        <item x="181"/>
+        <item x="182"/>
+        <item x="183"/>
+        <item x="184"/>
+        <item x="185"/>
+        <item x="186"/>
+        <item x="187"/>
+        <item x="188"/>
+        <item x="189"/>
+        <item x="190"/>
+        <item x="191"/>
+        <item x="192"/>
+        <item x="193"/>
+        <item x="194"/>
+        <item x="195"/>
+        <item x="196"/>
+        <item x="197"/>
+        <item x="198"/>
+        <item x="199"/>
+        <item x="200"/>
+        <item x="201"/>
+        <item x="202"/>
+        <item x="203"/>
+        <item x="204"/>
+        <item x="205"/>
+        <item x="206"/>
+        <item x="207"/>
+        <item x="208"/>
+        <item x="209"/>
+        <item x="210"/>
+        <item x="211"/>
+        <item x="212"/>
+        <item x="213"/>
+        <item x="214"/>
+        <item x="215"/>
+        <item x="216"/>
+        <item x="217"/>
+        <item x="218"/>
+        <item x="219"/>
+        <item x="220"/>
+        <item x="221"/>
+        <item x="222"/>
+        <item x="223"/>
+        <item x="224"/>
+        <item x="225"/>
+        <item x="226"/>
+        <item x="227"/>
+        <item x="228"/>
+        <item x="229"/>
+        <item x="230"/>
+        <item x="231"/>
+        <item x="232"/>
+        <item x="233"/>
+        <item x="234"/>
+        <item x="235"/>
+        <item x="236"/>
+        <item x="237"/>
+        <item x="238"/>
+        <item x="239"/>
+        <item x="240"/>
+        <item x="241"/>
+        <item x="242"/>
+        <item x="243"/>
+        <item x="244"/>
+        <item x="245"/>
+        <item x="246"/>
+        <item x="247"/>
+        <item x="248"/>
+        <item x="249"/>
+        <item x="250"/>
+        <item x="251"/>
+        <item x="252"/>
+        <item x="253"/>
+        <item x="254"/>
+        <item x="255"/>
+        <item x="256"/>
+        <item x="257"/>
+        <item x="258"/>
+        <item x="259"/>
+        <item x="260"/>
+        <item x="261"/>
+        <item x="262"/>
+        <item x="263"/>
+        <item x="264"/>
+        <item x="265"/>
+        <item x="266"/>
+        <item x="267"/>
+        <item x="268"/>
+        <item x="269"/>
+        <item x="270"/>
+        <item x="271"/>
+        <item x="272"/>
+        <item x="273"/>
+        <item x="274"/>
+        <item x="275"/>
+        <item x="276"/>
+        <item x="277"/>
+        <item x="278"/>
+        <item x="279"/>
+        <item x="280"/>
+        <item x="281"/>
+        <item x="282"/>
+        <item x="283"/>
+        <item x="284"/>
+        <item x="285"/>
+        <item x="286"/>
+        <item x="287"/>
+        <item x="288"/>
+        <item x="289"/>
+        <item x="290"/>
+        <item x="291"/>
+        <item x="292"/>
+        <item x="293"/>
+        <item x="294"/>
+        <item x="295"/>
+        <item x="296"/>
+        <item x="297"/>
+        <item x="298"/>
+        <item x="299"/>
+        <item x="300"/>
+        <item x="301"/>
+        <item x="302"/>
+        <item x="303"/>
+        <item x="304"/>
+        <item x="305"/>
+        <item x="306"/>
+        <item x="307"/>
+        <item x="308"/>
+        <item x="309"/>
+        <item x="310"/>
+        <item x="311"/>
+        <item x="312"/>
+        <item x="313"/>
+        <item x="314"/>
+        <item x="315"/>
+        <item x="316"/>
+        <item x="317"/>
+        <item x="318"/>
+        <item x="319"/>
+        <item x="320"/>
+        <item x="321"/>
+        <item x="322"/>
+        <item x="323"/>
+        <item x="324"/>
+        <item x="325"/>
+        <item x="326"/>
+        <item x="327"/>
+        <item x="328"/>
+        <item x="329"/>
+        <item x="330"/>
+        <item x="331"/>
+        <item x="332"/>
+        <item x="333"/>
+        <item x="334"/>
+        <item x="335"/>
+        <item x="336"/>
+        <item x="337"/>
+        <item x="338"/>
+        <item x="339"/>
+        <item x="340"/>
+        <item x="341"/>
+        <item x="342"/>
+        <item x="343"/>
+        <item x="344"/>
+        <item x="345"/>
+        <item x="346"/>
+        <item x="347"/>
+        <item x="348"/>
+        <item x="349"/>
+        <item x="350"/>
+        <item x="351"/>
+        <item x="352"/>
+        <item x="353"/>
+        <item x="354"/>
+        <item x="355"/>
+        <item x="356"/>
+        <item x="357"/>
+        <item x="358"/>
+        <item x="359"/>
+        <item x="360"/>
+        <item x="361"/>
+        <item x="362"/>
+        <item x="363"/>
+        <item x="364"/>
+        <item x="365"/>
+        <item x="366"/>
+        <item x="367"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="11">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item h="1" x="5"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="14"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="10" item="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count " fld="14" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="27">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="12">
+    <chartFormat chart="5" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="13" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="16">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="16">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="17">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="18">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" rowHeaderCaption="Client" colHeaderCaption="Month">
+  <location ref="A2:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="13">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="27">
+        <item x="18"/>
+        <item x="10"/>
+        <item x="19"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="6"/>
+        <item x="24"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="12"/>
+        <item x="1"/>
+        <item x="22"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="15"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="13"/>
+        <item x="23"/>
+        <item x="11"/>
+        <item x="9"/>
+        <item h="1" m="1" x="25"/>
+        <item h="1" x="0"/>
+        <item h="1" x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="24">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="EIM Platform Issues by Client - v7.5 onwards" fld="9" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="7">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="5">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5" rowHeaderCaption="Analysis Category">
   <location ref="A47:B53" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -23898,78 +24767,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Region" colHeaderCaption="Month">
-  <location ref="G2:H3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="13">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="12">
-        <item m="1" x="8"/>
-        <item m="1" x="9"/>
-        <item m="1" x="10"/>
-        <item m="1" x="6"/>
-        <item m="1" x="7"/>
-        <item h="1" m="1" x="5"/>
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item h="1" x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="1">
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="EIM Platform Issues by Region - v7.5 onwards" fld="9" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="4">
-    <format dxfId="7">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="6">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="5">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="4">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Analysis Category">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Analysis Category">
   <location ref="A25:B32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -24558,636 +25357,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10" rowHeaderCaption="Analysis Category">
-  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="16">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0">
-      <items count="368">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item x="52"/>
-        <item x="53"/>
-        <item x="54"/>
-        <item x="55"/>
-        <item x="56"/>
-        <item x="57"/>
-        <item x="58"/>
-        <item x="59"/>
-        <item x="60"/>
-        <item x="61"/>
-        <item x="62"/>
-        <item x="63"/>
-        <item x="64"/>
-        <item x="65"/>
-        <item x="66"/>
-        <item x="67"/>
-        <item x="68"/>
-        <item x="69"/>
-        <item x="70"/>
-        <item x="71"/>
-        <item x="72"/>
-        <item x="73"/>
-        <item x="74"/>
-        <item x="75"/>
-        <item x="76"/>
-        <item x="77"/>
-        <item x="78"/>
-        <item x="79"/>
-        <item x="80"/>
-        <item x="81"/>
-        <item x="82"/>
-        <item x="83"/>
-        <item x="84"/>
-        <item x="85"/>
-        <item x="86"/>
-        <item x="87"/>
-        <item x="88"/>
-        <item x="89"/>
-        <item x="90"/>
-        <item x="91"/>
-        <item x="92"/>
-        <item x="93"/>
-        <item x="94"/>
-        <item x="95"/>
-        <item x="96"/>
-        <item x="97"/>
-        <item x="98"/>
-        <item x="99"/>
-        <item x="100"/>
-        <item x="101"/>
-        <item x="102"/>
-        <item x="103"/>
-        <item x="104"/>
-        <item x="105"/>
-        <item x="106"/>
-        <item x="107"/>
-        <item x="108"/>
-        <item x="109"/>
-        <item x="110"/>
-        <item x="111"/>
-        <item x="112"/>
-        <item x="113"/>
-        <item x="114"/>
-        <item x="115"/>
-        <item x="116"/>
-        <item x="117"/>
-        <item x="118"/>
-        <item x="119"/>
-        <item x="120"/>
-        <item x="121"/>
-        <item x="122"/>
-        <item x="123"/>
-        <item x="124"/>
-        <item x="125"/>
-        <item x="126"/>
-        <item x="127"/>
-        <item x="128"/>
-        <item x="129"/>
-        <item x="130"/>
-        <item x="131"/>
-        <item x="132"/>
-        <item x="133"/>
-        <item x="134"/>
-        <item x="135"/>
-        <item x="136"/>
-        <item x="137"/>
-        <item x="138"/>
-        <item x="139"/>
-        <item x="140"/>
-        <item x="141"/>
-        <item x="142"/>
-        <item x="143"/>
-        <item x="144"/>
-        <item x="145"/>
-        <item x="146"/>
-        <item x="147"/>
-        <item x="148"/>
-        <item x="149"/>
-        <item x="150"/>
-        <item x="151"/>
-        <item x="152"/>
-        <item x="153"/>
-        <item x="154"/>
-        <item x="155"/>
-        <item x="156"/>
-        <item x="157"/>
-        <item x="158"/>
-        <item x="159"/>
-        <item x="160"/>
-        <item x="161"/>
-        <item x="162"/>
-        <item x="163"/>
-        <item x="164"/>
-        <item x="165"/>
-        <item x="166"/>
-        <item x="167"/>
-        <item x="168"/>
-        <item x="169"/>
-        <item x="170"/>
-        <item x="171"/>
-        <item x="172"/>
-        <item x="173"/>
-        <item x="174"/>
-        <item x="175"/>
-        <item x="176"/>
-        <item x="177"/>
-        <item x="178"/>
-        <item x="179"/>
-        <item x="180"/>
-        <item x="181"/>
-        <item x="182"/>
-        <item x="183"/>
-        <item x="184"/>
-        <item x="185"/>
-        <item x="186"/>
-        <item x="187"/>
-        <item x="188"/>
-        <item x="189"/>
-        <item x="190"/>
-        <item x="191"/>
-        <item x="192"/>
-        <item x="193"/>
-        <item x="194"/>
-        <item x="195"/>
-        <item x="196"/>
-        <item x="197"/>
-        <item x="198"/>
-        <item x="199"/>
-        <item x="200"/>
-        <item x="201"/>
-        <item x="202"/>
-        <item x="203"/>
-        <item x="204"/>
-        <item x="205"/>
-        <item x="206"/>
-        <item x="207"/>
-        <item x="208"/>
-        <item x="209"/>
-        <item x="210"/>
-        <item x="211"/>
-        <item x="212"/>
-        <item x="213"/>
-        <item x="214"/>
-        <item x="215"/>
-        <item x="216"/>
-        <item x="217"/>
-        <item x="218"/>
-        <item x="219"/>
-        <item x="220"/>
-        <item x="221"/>
-        <item x="222"/>
-        <item x="223"/>
-        <item x="224"/>
-        <item x="225"/>
-        <item x="226"/>
-        <item x="227"/>
-        <item x="228"/>
-        <item x="229"/>
-        <item x="230"/>
-        <item x="231"/>
-        <item x="232"/>
-        <item x="233"/>
-        <item x="234"/>
-        <item x="235"/>
-        <item x="236"/>
-        <item x="237"/>
-        <item x="238"/>
-        <item x="239"/>
-        <item x="240"/>
-        <item x="241"/>
-        <item x="242"/>
-        <item x="243"/>
-        <item x="244"/>
-        <item x="245"/>
-        <item x="246"/>
-        <item x="247"/>
-        <item x="248"/>
-        <item x="249"/>
-        <item x="250"/>
-        <item x="251"/>
-        <item x="252"/>
-        <item x="253"/>
-        <item x="254"/>
-        <item x="255"/>
-        <item x="256"/>
-        <item x="257"/>
-        <item x="258"/>
-        <item x="259"/>
-        <item x="260"/>
-        <item x="261"/>
-        <item x="262"/>
-        <item x="263"/>
-        <item x="264"/>
-        <item x="265"/>
-        <item x="266"/>
-        <item x="267"/>
-        <item x="268"/>
-        <item x="269"/>
-        <item x="270"/>
-        <item x="271"/>
-        <item x="272"/>
-        <item x="273"/>
-        <item x="274"/>
-        <item x="275"/>
-        <item x="276"/>
-        <item x="277"/>
-        <item x="278"/>
-        <item x="279"/>
-        <item x="280"/>
-        <item x="281"/>
-        <item x="282"/>
-        <item x="283"/>
-        <item x="284"/>
-        <item x="285"/>
-        <item x="286"/>
-        <item x="287"/>
-        <item x="288"/>
-        <item x="289"/>
-        <item x="290"/>
-        <item x="291"/>
-        <item x="292"/>
-        <item x="293"/>
-        <item x="294"/>
-        <item x="295"/>
-        <item x="296"/>
-        <item x="297"/>
-        <item x="298"/>
-        <item x="299"/>
-        <item x="300"/>
-        <item x="301"/>
-        <item x="302"/>
-        <item x="303"/>
-        <item x="304"/>
-        <item x="305"/>
-        <item x="306"/>
-        <item x="307"/>
-        <item x="308"/>
-        <item x="309"/>
-        <item x="310"/>
-        <item x="311"/>
-        <item x="312"/>
-        <item x="313"/>
-        <item x="314"/>
-        <item x="315"/>
-        <item x="316"/>
-        <item x="317"/>
-        <item x="318"/>
-        <item x="319"/>
-        <item x="320"/>
-        <item x="321"/>
-        <item x="322"/>
-        <item x="323"/>
-        <item x="324"/>
-        <item x="325"/>
-        <item x="326"/>
-        <item x="327"/>
-        <item x="328"/>
-        <item x="329"/>
-        <item x="330"/>
-        <item x="331"/>
-        <item x="332"/>
-        <item x="333"/>
-        <item x="334"/>
-        <item x="335"/>
-        <item x="336"/>
-        <item x="337"/>
-        <item x="338"/>
-        <item x="339"/>
-        <item x="340"/>
-        <item x="341"/>
-        <item x="342"/>
-        <item x="343"/>
-        <item x="344"/>
-        <item x="345"/>
-        <item x="346"/>
-        <item x="347"/>
-        <item x="348"/>
-        <item x="349"/>
-        <item x="350"/>
-        <item x="351"/>
-        <item x="352"/>
-        <item x="353"/>
-        <item x="354"/>
-        <item x="355"/>
-        <item x="356"/>
-        <item x="357"/>
-        <item x="358"/>
-        <item x="359"/>
-        <item x="360"/>
-        <item x="361"/>
-        <item x="362"/>
-        <item x="363"/>
-        <item x="364"/>
-        <item x="365"/>
-        <item x="366"/>
-        <item x="367"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="11">
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item h="1" x="5"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0">
-      <items count="14">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="14"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="10" item="0" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count " fld="14" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="27">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="12">
-    <chartFormat chart="5" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="13" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="16">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="16">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="17">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="18">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" rowHeaderCaption="Client" colHeaderCaption="Month">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" rowHeaderCaption="Client" colHeaderCaption="Month">
   <location ref="A2:E28" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -25804,7 +25975,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="G2:K9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -26312,7 +26483,408 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5" rowHeaderCaption="Analysis Category">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Analysis Category">
+  <location ref="A25:B32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="17">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="12">
+        <item x="3"/>
+        <item h="1" x="6"/>
+        <item h="1" x="8"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item h="1" x="7"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="12"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="8" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count" fld="12" subtotal="count" baseField="9" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="9">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Analysis Category">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="17">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="12">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item h="1" x="6"/>
+        <item h="1" x="8"/>
+        <item x="5"/>
+        <item h="1" x="7"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="12"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="8" item="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count" fld="12" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="8">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="12" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5" rowHeaderCaption="Analysis Category">
   <location ref="A47:B53" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -26554,528 +27126,43 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Analysis Category">
-  <location ref="A25:B32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Region" colHeaderCaption="Month">
+  <location ref="G2:H3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="17">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="12">
-        <item x="3"/>
-        <item h="1" x="6"/>
-        <item h="1" x="8"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item h="1" x="7"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="12"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="8" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count" fld="12" subtotal="count" baseField="9" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="9">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Analysis Category">
-  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="13">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="17">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="12">
-        <item x="3"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item h="1" x="6"/>
-        <item h="1" x="8"/>
-        <item x="5"/>
-        <item h="1" x="7"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="12"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="8" item="0" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count" fld="12" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="8">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="8">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="12" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" rowHeaderCaption="Client" colHeaderCaption="Month">
-  <location ref="A2:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="13">
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="27">
-        <item x="18"/>
-        <item x="10"/>
-        <item x="19"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="6"/>
-        <item x="24"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item x="12"/>
-        <item x="1"/>
-        <item x="22"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="15"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="13"/>
-        <item x="23"/>
-        <item x="11"/>
-        <item x="9"/>
-        <item h="1" m="1" x="25"/>
+        <item m="1" x="8"/>
+        <item m="1" x="9"/>
+        <item m="1" x="10"/>
+        <item m="1" x="6"/>
+        <item m="1" x="7"/>
+        <item h="1" m="1" x="5"/>
         <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
         <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="5"/>
+    <field x="6"/>
   </rowFields>
-  <rowItems count="24">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
+  <rowItems count="1">
     <i t="grand">
       <x/>
     </i>
@@ -27084,7 +27171,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="EIM Platform Issues by Client - v7.5 onwards" fld="9" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="EIM Platform Issues by Region - v7.5 onwards" fld="9" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
     <format dxfId="3">
@@ -34609,11 +34696,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R438"/>
+  <dimension ref="A1:R449"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A417" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G433" sqref="G433"/>
+      <selection pane="bottomLeft" activeCell="A446" sqref="A446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52024,6 +52111,448 @@
         <v>326</v>
       </c>
       <c r="N438" s="44"/>
+    </row>
+    <row r="439" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A439" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B439" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C439" s="7" t="s">
+        <v>1901</v>
+      </c>
+      <c r="D439" s="7" t="s">
+        <v>1902</v>
+      </c>
+      <c r="E439" s="45" t="s">
+        <v>1903</v>
+      </c>
+      <c r="F439" s="30" t="s">
+        <v>1049</v>
+      </c>
+      <c r="G439" s="30" t="s">
+        <v>1273</v>
+      </c>
+      <c r="H439" s="7"/>
+      <c r="I439" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="J439" s="33">
+        <v>44805</v>
+      </c>
+      <c r="K439" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="L439" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="M439" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="N439" s="44" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="440" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A440" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B440" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C440" s="7" t="s">
+        <v>1904</v>
+      </c>
+      <c r="D440" s="7" t="s">
+        <v>1905</v>
+      </c>
+      <c r="E440" s="45" t="s">
+        <v>1906</v>
+      </c>
+      <c r="F440" s="30" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G440" s="30" t="s">
+        <v>1271</v>
+      </c>
+      <c r="H440" s="7"/>
+      <c r="I440" s="7">
+        <v>7.2</v>
+      </c>
+      <c r="J440" s="33">
+        <v>44805</v>
+      </c>
+      <c r="K440" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L440" s="44" t="s">
+        <v>508</v>
+      </c>
+      <c r="M440" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="N440" s="44"/>
+    </row>
+    <row r="441" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A441" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B441" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C441" s="7" t="s">
+        <v>1907</v>
+      </c>
+      <c r="D441" s="7" t="s">
+        <v>1908</v>
+      </c>
+      <c r="E441" s="45" t="s">
+        <v>1836</v>
+      </c>
+      <c r="F441" s="45" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G441" s="45" t="s">
+        <v>1271</v>
+      </c>
+      <c r="H441" s="7"/>
+      <c r="I441" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="J441" s="33">
+        <v>44805</v>
+      </c>
+      <c r="K441" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L441" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="M441" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="N441" s="44"/>
+    </row>
+    <row r="442" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A442" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B442" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C442" s="7" t="s">
+        <v>1909</v>
+      </c>
+      <c r="D442" s="7" t="s">
+        <v>1910</v>
+      </c>
+      <c r="E442" s="45" t="s">
+        <v>537</v>
+      </c>
+      <c r="F442" s="45" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G442" s="45" t="s">
+        <v>1271</v>
+      </c>
+      <c r="H442" s="7"/>
+      <c r="I442" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="J442" s="33">
+        <v>44805</v>
+      </c>
+      <c r="K442" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L442" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="M442" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="N442" s="44"/>
+    </row>
+    <row r="443" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A443" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B443" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C443" s="7" t="s">
+        <v>1911</v>
+      </c>
+      <c r="D443" s="7" t="s">
+        <v>1912</v>
+      </c>
+      <c r="E443" s="45" t="s">
+        <v>1913</v>
+      </c>
+      <c r="F443" s="30" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G443" s="30" t="s">
+        <v>1270</v>
+      </c>
+      <c r="H443" s="7"/>
+      <c r="I443" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="J443" s="33">
+        <v>44805</v>
+      </c>
+      <c r="K443" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="L443" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="M443" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="N443" s="44"/>
+    </row>
+    <row r="444" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A444" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B444" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C444" s="7" t="s">
+        <v>1914</v>
+      </c>
+      <c r="D444" s="7" t="s">
+        <v>1915</v>
+      </c>
+      <c r="E444" s="45" t="s">
+        <v>1916</v>
+      </c>
+      <c r="F444" s="27" t="s">
+        <v>992</v>
+      </c>
+      <c r="G444" s="27" t="s">
+        <v>1273</v>
+      </c>
+      <c r="H444" s="7"/>
+      <c r="I444" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="J444" s="33">
+        <v>44805</v>
+      </c>
+      <c r="K444" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L444" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="M444" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="N444" s="44"/>
+    </row>
+    <row r="445" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A445" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B445" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C445" s="7" t="s">
+        <v>1917</v>
+      </c>
+      <c r="D445" s="7" t="s">
+        <v>1918</v>
+      </c>
+      <c r="E445" s="45" t="s">
+        <v>1919</v>
+      </c>
+      <c r="F445" s="30" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G445" s="30" t="s">
+        <v>1270</v>
+      </c>
+      <c r="H445" s="7"/>
+      <c r="I445" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="J445" s="33">
+        <v>44805</v>
+      </c>
+      <c r="K445" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L445" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="M445" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="N445" s="44"/>
+    </row>
+    <row r="446" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A446" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B446" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C446" s="7" t="s">
+        <v>1920</v>
+      </c>
+      <c r="D446" s="7" t="s">
+        <v>1921</v>
+      </c>
+      <c r="E446" s="45" t="s">
+        <v>1903</v>
+      </c>
+      <c r="F446" s="30" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G446" s="30" t="s">
+        <v>1270</v>
+      </c>
+      <c r="H446" s="7"/>
+      <c r="I446" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="J446" s="33">
+        <v>44805</v>
+      </c>
+      <c r="K446" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="L446" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="M446" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="N446" s="44"/>
+    </row>
+    <row r="447" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A447" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B447" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C447" s="7" t="s">
+        <v>1922</v>
+      </c>
+      <c r="D447" s="7" t="s">
+        <v>1923</v>
+      </c>
+      <c r="E447" s="45" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F447" s="45" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G447" s="45" t="s">
+        <v>1271</v>
+      </c>
+      <c r="H447" s="7"/>
+      <c r="I447" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="J447" s="33">
+        <v>44805</v>
+      </c>
+      <c r="K447" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L447" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="M447" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="N447" s="44"/>
+    </row>
+    <row r="448" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A448" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B448" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C448" s="7" t="s">
+        <v>1925</v>
+      </c>
+      <c r="D448" s="7" t="s">
+        <v>1926</v>
+      </c>
+      <c r="E448" s="45" t="s">
+        <v>537</v>
+      </c>
+      <c r="F448" s="45" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G448" s="45" t="s">
+        <v>1271</v>
+      </c>
+      <c r="H448" s="7"/>
+      <c r="I448" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="J448" s="33">
+        <v>44805</v>
+      </c>
+      <c r="K448" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L448" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="M448" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="N448" s="44"/>
+    </row>
+    <row r="449" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A449" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B449" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C449" s="7" t="s">
+        <v>1927</v>
+      </c>
+      <c r="D449" s="7" t="s">
+        <v>1928</v>
+      </c>
+      <c r="E449" s="45" t="s">
+        <v>1929</v>
+      </c>
+      <c r="F449" s="30" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G449" s="30" t="s">
+        <v>1271</v>
+      </c>
+      <c r="H449" s="7"/>
+      <c r="I449" s="7">
+        <v>7.2</v>
+      </c>
+      <c r="J449" s="33">
+        <v>44805</v>
+      </c>
+      <c r="K449" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L449" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="M449" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="N449" s="44"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M380"/>

</xml_diff>